<commit_message>
Testando a implementação dos Backups
</commit_message>
<xml_diff>
--- a/storage/listaRDMARCAS.xlsx
+++ b/storage/listaRDMARCAS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,293 +470,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>31/03/2000</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>5525.5</v>
-      </c>
-      <c r="C2" t="n">
-        <v>5525.5</v>
-      </c>
-      <c r="D2" t="n">
-        <v>6605.7</v>
-      </c>
-      <c r="E2" t="n">
-        <v>6605.7</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1080.2</v>
-      </c>
-      <c r="G2" t="n">
-        <v>119.55</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>31/03/2000</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>5525.5</v>
-      </c>
-      <c r="C3" t="n">
-        <v>11051</v>
-      </c>
-      <c r="D3" t="n">
-        <v>6605.7</v>
-      </c>
-      <c r="E3" t="n">
-        <v>13211.4</v>
-      </c>
-      <c r="F3" t="n">
-        <v>2160.4</v>
-      </c>
-      <c r="G3" t="n">
-        <v>119.55</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>31/03/2000</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>5525.5</v>
-      </c>
-      <c r="C4" t="n">
-        <v>16576.5</v>
-      </c>
-      <c r="D4" t="n">
-        <v>6605.7</v>
-      </c>
-      <c r="E4" t="n">
-        <v>19817.1</v>
-      </c>
-      <c r="F4" t="n">
-        <v>3240.6</v>
-      </c>
-      <c r="G4" t="n">
-        <v>119.55</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>31/03/2000</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>5525.5</v>
-      </c>
-      <c r="C5" t="n">
-        <v>22102</v>
-      </c>
-      <c r="D5" t="n">
-        <v>6605.7</v>
-      </c>
-      <c r="E5" t="n">
-        <v>26422.8</v>
-      </c>
-      <c r="F5" t="n">
-        <v>4320.8</v>
-      </c>
-      <c r="G5" t="n">
-        <v>119.55</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>31/03/2000</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>5525.5</v>
-      </c>
-      <c r="C6" t="n">
-        <v>27627.5</v>
-      </c>
-      <c r="D6" t="n">
-        <v>6605.7</v>
-      </c>
-      <c r="E6" t="n">
-        <v>33028.5</v>
-      </c>
-      <c r="F6" t="n">
-        <v>5401</v>
-      </c>
-      <c r="G6" t="n">
-        <v>119.55</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>31/03/2000</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>5525.5</v>
-      </c>
-      <c r="C7" t="n">
-        <v>33153</v>
-      </c>
-      <c r="D7" t="n">
-        <v>6605.7</v>
-      </c>
-      <c r="E7" t="n">
-        <v>39634.2</v>
-      </c>
-      <c r="F7" t="n">
-        <v>6481.2</v>
-      </c>
-      <c r="G7" t="n">
-        <v>119.55</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>31/03/2000</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>5525.5</v>
-      </c>
-      <c r="C8" t="n">
-        <v>38678.5</v>
-      </c>
-      <c r="D8" t="n">
-        <v>6605.7</v>
-      </c>
-      <c r="E8" t="n">
-        <v>46239.9</v>
-      </c>
-      <c r="F8" t="n">
-        <v>7561.4</v>
-      </c>
-      <c r="G8" t="n">
-        <v>119.55</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>31/03/2000</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>5525.5</v>
-      </c>
-      <c r="C9" t="n">
-        <v>44204</v>
-      </c>
-      <c r="D9" t="n">
-        <v>6605.7</v>
-      </c>
-      <c r="E9" t="n">
-        <v>52845.6</v>
-      </c>
-      <c r="F9" t="n">
-        <v>8641.6</v>
-      </c>
-      <c r="G9" t="n">
-        <v>119.55</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>31/03/2000</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>5525.5</v>
-      </c>
-      <c r="C10" t="n">
-        <v>49729.5</v>
-      </c>
-      <c r="D10" t="n">
-        <v>6605.7</v>
-      </c>
-      <c r="E10" t="n">
-        <v>59451.3</v>
-      </c>
-      <c r="F10" t="n">
-        <v>9721.799999999999</v>
-      </c>
-      <c r="G10" t="n">
-        <v>119.55</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>31/03/2000</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>5525.5</v>
-      </c>
-      <c r="C11" t="n">
-        <v>55255</v>
-      </c>
-      <c r="D11" t="n">
-        <v>6605.7</v>
-      </c>
-      <c r="E11" t="n">
-        <v>66057</v>
-      </c>
-      <c r="F11" t="n">
-        <v>10802</v>
-      </c>
-      <c r="G11" t="n">
-        <v>119.55</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>31/03/2000</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>5525.50</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>60780.50</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>6605.70</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>72662.70</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>11882.20</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>119.55</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Está sendo implementado variáveis de fontes para diferentes plataformas android/desktop
</commit_message>
<xml_diff>
--- a/storage/listaRDMARCAS.xlsx
+++ b/storage/listaRDMARCAS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -751,35 +751,23 @@
           <t>16/07/2023</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>6800.00</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>61302.40</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>9804.88</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>64304.88</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>3002.48</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>104.90</t>
-        </is>
+      <c r="B13" t="n">
+        <v>6800</v>
+      </c>
+      <c r="C13" t="n">
+        <v>61302.4</v>
+      </c>
+      <c r="D13" t="n">
+        <v>9804.879999999999</v>
+      </c>
+      <c r="E13" t="n">
+        <v>64304.88</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3002.48</v>
+      </c>
+      <c r="G13" t="n">
+        <v>104.9</v>
       </c>
     </row>
     <row r="14">
@@ -788,35 +776,23 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>66302.40</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>69304.88</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>3002.48</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>104.53</t>
-        </is>
+      <c r="B14" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C14" t="n">
+        <v>66302.39999999999</v>
+      </c>
+      <c r="D14" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E14" t="n">
+        <v>69304.88</v>
+      </c>
+      <c r="F14" t="n">
+        <v>3002.48</v>
+      </c>
+      <c r="G14" t="n">
+        <v>104.53</v>
       </c>
     </row>
     <row r="15">
@@ -825,35 +801,23 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>71302.40</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>74304.88</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>3002.48</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>104.21</t>
-        </is>
+      <c r="B15" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C15" t="n">
+        <v>71302.39999999999</v>
+      </c>
+      <c r="D15" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E15" t="n">
+        <v>74304.88</v>
+      </c>
+      <c r="F15" t="n">
+        <v>3002.48</v>
+      </c>
+      <c r="G15" t="n">
+        <v>104.21</v>
       </c>
     </row>
     <row r="16">
@@ -862,35 +826,23 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>76302.40</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>79304.88</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>3002.48</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>103.93</t>
-        </is>
+      <c r="B16" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C16" t="n">
+        <v>76302.39999999999</v>
+      </c>
+      <c r="D16" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E16" t="n">
+        <v>79304.88</v>
+      </c>
+      <c r="F16" t="n">
+        <v>3002.48</v>
+      </c>
+      <c r="G16" t="n">
+        <v>103.93</v>
       </c>
     </row>
     <row r="17">
@@ -899,35 +851,23 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>81302.40</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>84304.88</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>3002.48</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>103.69</t>
-        </is>
+      <c r="B17" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C17" t="n">
+        <v>81302.39999999999</v>
+      </c>
+      <c r="D17" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E17" t="n">
+        <v>84304.88</v>
+      </c>
+      <c r="F17" t="n">
+        <v>3002.48</v>
+      </c>
+      <c r="G17" t="n">
+        <v>103.69</v>
       </c>
     </row>
     <row r="18">
@@ -936,35 +876,23 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>86302.40</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>89304.88</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>3002.48</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>103.48</t>
-        </is>
+      <c r="B18" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C18" t="n">
+        <v>86302.39999999999</v>
+      </c>
+      <c r="D18" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E18" t="n">
+        <v>89304.88</v>
+      </c>
+      <c r="F18" t="n">
+        <v>3002.48</v>
+      </c>
+      <c r="G18" t="n">
+        <v>103.48</v>
       </c>
     </row>
     <row r="19">
@@ -973,35 +901,23 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>91302.40</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>94304.88</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>3002.48</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>103.29</t>
-        </is>
+      <c r="B19" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C19" t="n">
+        <v>91302.39999999999</v>
+      </c>
+      <c r="D19" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E19" t="n">
+        <v>94304.88</v>
+      </c>
+      <c r="F19" t="n">
+        <v>3002.48</v>
+      </c>
+      <c r="G19" t="n">
+        <v>103.29</v>
       </c>
     </row>
     <row r="20">
@@ -1010,35 +926,23 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>96302.40</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>99304.88</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>3002.48</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>103.12</t>
-        </is>
+      <c r="B20" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C20" t="n">
+        <v>96302.39999999999</v>
+      </c>
+      <c r="D20" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E20" t="n">
+        <v>99304.88</v>
+      </c>
+      <c r="F20" t="n">
+        <v>3002.48</v>
+      </c>
+      <c r="G20" t="n">
+        <v>103.12</v>
       </c>
     </row>
     <row r="21">
@@ -1047,35 +951,23 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>101302.40</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>104304.88</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>3002.48</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>102.96</t>
-        </is>
+      <c r="B21" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C21" t="n">
+        <v>101302.4</v>
+      </c>
+      <c r="D21" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E21" t="n">
+        <v>104304.88</v>
+      </c>
+      <c r="F21" t="n">
+        <v>3002.48</v>
+      </c>
+      <c r="G21" t="n">
+        <v>102.96</v>
       </c>
     </row>
     <row r="22">
@@ -1084,35 +976,23 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>106302.40</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>109304.88</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>3002.48</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>102.82</t>
-        </is>
+      <c r="B22" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C22" t="n">
+        <v>106302.4</v>
+      </c>
+      <c r="D22" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E22" t="n">
+        <v>109304.88</v>
+      </c>
+      <c r="F22" t="n">
+        <v>3002.48</v>
+      </c>
+      <c r="G22" t="n">
+        <v>102.82</v>
       </c>
     </row>
     <row r="23">
@@ -1121,35 +1001,23 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>111302.40</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>114304.88</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>3002.48</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>102.70</t>
-        </is>
+      <c r="B23" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C23" t="n">
+        <v>111302.4</v>
+      </c>
+      <c r="D23" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E23" t="n">
+        <v>114304.88</v>
+      </c>
+      <c r="F23" t="n">
+        <v>3002.48</v>
+      </c>
+      <c r="G23" t="n">
+        <v>102.7</v>
       </c>
     </row>
     <row r="24">
@@ -1158,35 +1026,23 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>116302.40</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>119304.88</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>3002.48</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>102.58</t>
-        </is>
+      <c r="B24" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C24" t="n">
+        <v>116302.4</v>
+      </c>
+      <c r="D24" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E24" t="n">
+        <v>119304.88</v>
+      </c>
+      <c r="F24" t="n">
+        <v>3002.48</v>
+      </c>
+      <c r="G24" t="n">
+        <v>102.58</v>
       </c>
     </row>
     <row r="25">
@@ -1195,35 +1051,23 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>121302.40</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>124304.88</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>3002.48</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>102.48</t>
-        </is>
+      <c r="B25" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C25" t="n">
+        <v>121302.4</v>
+      </c>
+      <c r="D25" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E25" t="n">
+        <v>124304.88</v>
+      </c>
+      <c r="F25" t="n">
+        <v>3002.48</v>
+      </c>
+      <c r="G25" t="n">
+        <v>102.48</v>
       </c>
     </row>
     <row r="26">
@@ -1232,35 +1076,23 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>126302.40</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>129304.88</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>3002.48</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>102.38</t>
-        </is>
+      <c r="B26" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C26" t="n">
+        <v>126302.4</v>
+      </c>
+      <c r="D26" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E26" t="n">
+        <v>129304.88</v>
+      </c>
+      <c r="F26" t="n">
+        <v>3002.48</v>
+      </c>
+      <c r="G26" t="n">
+        <v>102.38</v>
       </c>
     </row>
     <row r="27">
@@ -1269,35 +1101,23 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>131302.40</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>134304.88</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>3002.48</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>102.29</t>
-        </is>
+      <c r="B27" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C27" t="n">
+        <v>131302.4</v>
+      </c>
+      <c r="D27" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E27" t="n">
+        <v>134304.88</v>
+      </c>
+      <c r="F27" t="n">
+        <v>3002.48</v>
+      </c>
+      <c r="G27" t="n">
+        <v>102.29</v>
       </c>
     </row>
     <row r="28">
@@ -1306,35 +1126,23 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>136302.40</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>139304.88</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>3002.48</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>102.20</t>
-        </is>
+      <c r="B28" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C28" t="n">
+        <v>136302.4</v>
+      </c>
+      <c r="D28" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E28" t="n">
+        <v>139304.88</v>
+      </c>
+      <c r="F28" t="n">
+        <v>3002.48</v>
+      </c>
+      <c r="G28" t="n">
+        <v>102.2</v>
       </c>
     </row>
     <row r="29">
@@ -1343,35 +1151,23 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>141302.40</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>144304.88</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>3002.48</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>102.12</t>
-        </is>
+      <c r="B29" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C29" t="n">
+        <v>141302.4</v>
+      </c>
+      <c r="D29" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E29" t="n">
+        <v>144304.88</v>
+      </c>
+      <c r="F29" t="n">
+        <v>3002.48</v>
+      </c>
+      <c r="G29" t="n">
+        <v>102.12</v>
       </c>
     </row>
     <row r="30">
@@ -1380,35 +1176,23 @@
           <t>30/08/2001</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>6000.00</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>147302.40</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>8000.80</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>152305.68</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>5003.28</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>103.40</t>
-        </is>
+      <c r="B30" t="n">
+        <v>6000</v>
+      </c>
+      <c r="C30" t="n">
+        <v>147302.4</v>
+      </c>
+      <c r="D30" t="n">
+        <v>8000.8</v>
+      </c>
+      <c r="E30" t="n">
+        <v>152305.68</v>
+      </c>
+      <c r="F30" t="n">
+        <v>5003.28</v>
+      </c>
+      <c r="G30" t="n">
+        <v>103.4</v>
       </c>
     </row>
     <row r="31">
@@ -1417,34 +1201,59 @@
           <t>50/08/2000</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>3000.86</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>150303.26</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>6580.60</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>158886.28</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>8583.02</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>105.71</t>
+      <c r="B31" t="n">
+        <v>3000.86</v>
+      </c>
+      <c r="C31" t="n">
+        <v>150303.26</v>
+      </c>
+      <c r="D31" t="n">
+        <v>6580.6</v>
+      </c>
+      <c r="E31" t="n">
+        <v>158886.28</v>
+      </c>
+      <c r="F31" t="n">
+        <v>8583.02</v>
+      </c>
+      <c r="G31" t="n">
+        <v>105.71</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>30/08/5200</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>35600.00</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>185903.26</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>64641.00</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>223527.28</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>37624.02</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>120.24</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajustes de fontes para desktop/android
</commit_message>
<xml_diff>
--- a/storage/listaRDMARCAS.xlsx
+++ b/storage/listaRDMARCAS.xlsx
@@ -548,26 +548,38 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>14/07/2023</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>6000</v>
-      </c>
-      <c r="C5" t="n">
-        <v>27800.6</v>
-      </c>
-      <c r="D5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="E5" t="n">
-        <v>34500</v>
-      </c>
-      <c r="F5" t="n">
-        <v>6699.4</v>
-      </c>
-      <c r="G5" t="n">
-        <v>124.1</v>
+          <t>31/08/0800</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>6800.00</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>28600.60</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>9000.00</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>28500.00</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>100.60</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>99.65</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -576,23 +588,35 @@
           <t>14/07/2023</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>6700</v>
-      </c>
-      <c r="C6" t="n">
-        <v>34500.6</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>34500</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="G6" t="n">
-        <v>100</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>6700.00</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>35300.60</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>28500.00</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>6800.60</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>80.74</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -601,23 +625,35 @@
           <t>14/07/2023</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C7" t="n">
-        <v>34501.2</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>34500</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="G7" t="n">
-        <v>100</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0.60</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>35301.20</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>28500.00</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>6801.20</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>80.73</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -626,23 +662,35 @@
           <t>14/07/2023</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="C8" t="n">
-        <v>34502.4</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>34500</v>
-      </c>
-      <c r="F8" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="G8" t="n">
-        <v>99.98999999999999</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1.20</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>35302.40</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>28500.00</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>6802.40</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>80.73</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -651,23 +699,35 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C9" t="n">
-        <v>39502.4</v>
-      </c>
-      <c r="D9" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E9" t="n">
-        <v>39500</v>
-      </c>
-      <c r="F9" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="G9" t="n">
-        <v>99.98999999999999</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>40302.40</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>33500.00</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>6802.40</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>83.12</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -676,23 +736,35 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C10" t="n">
-        <v>44502.4</v>
-      </c>
-      <c r="D10" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E10" t="n">
-        <v>44500</v>
-      </c>
-      <c r="F10" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="G10" t="n">
-        <v>99.98999999999999</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>45302.40</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>38500.00</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>6802.40</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>84.98</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -701,23 +773,35 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C11" t="n">
-        <v>49502.4</v>
-      </c>
-      <c r="D11" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E11" t="n">
-        <v>49500</v>
-      </c>
-      <c r="F11" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="G11" t="n">
-        <v>100</v>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>50302.40</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>43500.00</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>6802.40</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>86.48</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -726,23 +810,35 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C12" t="n">
-        <v>54502.4</v>
-      </c>
-      <c r="D12" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E12" t="n">
-        <v>54500</v>
-      </c>
-      <c r="F12" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="G12" t="n">
-        <v>100</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>55302.40</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>48500.00</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>6802.40</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>87.70</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -751,23 +847,35 @@
           <t>16/07/2023</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>6800</v>
-      </c>
-      <c r="C13" t="n">
-        <v>61302.4</v>
-      </c>
-      <c r="D13" t="n">
-        <v>9804.879999999999</v>
-      </c>
-      <c r="E13" t="n">
-        <v>64304.88</v>
-      </c>
-      <c r="F13" t="n">
-        <v>3002.48</v>
-      </c>
-      <c r="G13" t="n">
-        <v>104.9</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>6800.00</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>62102.40</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>9804.88</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>58304.88</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>3797.52</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>93.89</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -776,23 +884,35 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C14" t="n">
-        <v>66302.39999999999</v>
-      </c>
-      <c r="D14" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E14" t="n">
-        <v>69304.88</v>
-      </c>
-      <c r="F14" t="n">
-        <v>3002.48</v>
-      </c>
-      <c r="G14" t="n">
-        <v>104.53</v>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>67102.40</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>63304.88</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>3797.52</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>94.34</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -801,23 +921,35 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C15" t="n">
-        <v>71302.39999999999</v>
-      </c>
-      <c r="D15" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E15" t="n">
-        <v>74304.88</v>
-      </c>
-      <c r="F15" t="n">
-        <v>3002.48</v>
-      </c>
-      <c r="G15" t="n">
-        <v>104.21</v>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>72102.40</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>68304.88</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>3797.52</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>94.73</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -826,23 +958,35 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B16" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C16" t="n">
-        <v>76302.39999999999</v>
-      </c>
-      <c r="D16" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E16" t="n">
-        <v>79304.88</v>
-      </c>
-      <c r="F16" t="n">
-        <v>3002.48</v>
-      </c>
-      <c r="G16" t="n">
-        <v>103.93</v>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>77102.40</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>73304.88</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>3797.52</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>95.07</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -851,23 +995,35 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B17" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C17" t="n">
-        <v>81302.39999999999</v>
-      </c>
-      <c r="D17" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E17" t="n">
-        <v>84304.88</v>
-      </c>
-      <c r="F17" t="n">
-        <v>3002.48</v>
-      </c>
-      <c r="G17" t="n">
-        <v>103.69</v>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>82102.40</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>78304.88</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>3797.52</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>95.37</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -876,23 +1032,35 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C18" t="n">
-        <v>86302.39999999999</v>
-      </c>
-      <c r="D18" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E18" t="n">
-        <v>89304.88</v>
-      </c>
-      <c r="F18" t="n">
-        <v>3002.48</v>
-      </c>
-      <c r="G18" t="n">
-        <v>103.48</v>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>87102.40</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>83304.88</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>3797.52</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>95.64</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -901,23 +1069,35 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B19" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C19" t="n">
-        <v>91302.39999999999</v>
-      </c>
-      <c r="D19" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E19" t="n">
-        <v>94304.88</v>
-      </c>
-      <c r="F19" t="n">
-        <v>3002.48</v>
-      </c>
-      <c r="G19" t="n">
-        <v>103.29</v>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>92102.40</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>88304.88</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>3797.52</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>95.88</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -926,23 +1106,35 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B20" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C20" t="n">
-        <v>96302.39999999999</v>
-      </c>
-      <c r="D20" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E20" t="n">
-        <v>99304.88</v>
-      </c>
-      <c r="F20" t="n">
-        <v>3002.48</v>
-      </c>
-      <c r="G20" t="n">
-        <v>103.12</v>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>97102.40</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>93304.88</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>3797.52</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>96.09</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -951,23 +1143,35 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B21" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C21" t="n">
-        <v>101302.4</v>
-      </c>
-      <c r="D21" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E21" t="n">
-        <v>104304.88</v>
-      </c>
-      <c r="F21" t="n">
-        <v>3002.48</v>
-      </c>
-      <c r="G21" t="n">
-        <v>102.96</v>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>102102.40</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>98304.88</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>3797.52</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>96.28</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -976,23 +1180,35 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B22" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C22" t="n">
-        <v>106302.4</v>
-      </c>
-      <c r="D22" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E22" t="n">
-        <v>109304.88</v>
-      </c>
-      <c r="F22" t="n">
-        <v>3002.48</v>
-      </c>
-      <c r="G22" t="n">
-        <v>102.82</v>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>107102.40</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>103304.88</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>3797.52</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>96.45</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -1001,23 +1217,35 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B23" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C23" t="n">
-        <v>111302.4</v>
-      </c>
-      <c r="D23" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E23" t="n">
-        <v>114304.88</v>
-      </c>
-      <c r="F23" t="n">
-        <v>3002.48</v>
-      </c>
-      <c r="G23" t="n">
-        <v>102.7</v>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>112102.40</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>108304.88</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>3797.52</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>96.61</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -1026,23 +1254,35 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B24" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C24" t="n">
-        <v>116302.4</v>
-      </c>
-      <c r="D24" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E24" t="n">
-        <v>119304.88</v>
-      </c>
-      <c r="F24" t="n">
-        <v>3002.48</v>
-      </c>
-      <c r="G24" t="n">
-        <v>102.58</v>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>117102.40</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>113304.88</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>3797.52</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>96.76</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -1051,23 +1291,35 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B25" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C25" t="n">
-        <v>121302.4</v>
-      </c>
-      <c r="D25" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E25" t="n">
-        <v>124304.88</v>
-      </c>
-      <c r="F25" t="n">
-        <v>3002.48</v>
-      </c>
-      <c r="G25" t="n">
-        <v>102.48</v>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>122102.40</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>118304.88</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>3797.52</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>96.89</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -1076,23 +1328,35 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B26" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C26" t="n">
-        <v>126302.4</v>
-      </c>
-      <c r="D26" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E26" t="n">
-        <v>129304.88</v>
-      </c>
-      <c r="F26" t="n">
-        <v>3002.48</v>
-      </c>
-      <c r="G26" t="n">
-        <v>102.38</v>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>127102.40</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>123304.88</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>3797.52</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>97.01</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -1101,23 +1365,35 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B27" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C27" t="n">
-        <v>131302.4</v>
-      </c>
-      <c r="D27" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E27" t="n">
-        <v>134304.88</v>
-      </c>
-      <c r="F27" t="n">
-        <v>3002.48</v>
-      </c>
-      <c r="G27" t="n">
-        <v>102.29</v>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>132102.40</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>128304.88</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>3797.52</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>97.13</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -1126,23 +1402,35 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B28" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C28" t="n">
-        <v>136302.4</v>
-      </c>
-      <c r="D28" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E28" t="n">
-        <v>139304.88</v>
-      </c>
-      <c r="F28" t="n">
-        <v>3002.48</v>
-      </c>
-      <c r="G28" t="n">
-        <v>102.2</v>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>137102.40</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>133304.88</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>3797.52</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>97.23</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -1151,23 +1439,35 @@
           <t>15/07/2023</t>
         </is>
       </c>
-      <c r="B29" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C29" t="n">
-        <v>141302.4</v>
-      </c>
-      <c r="D29" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E29" t="n">
-        <v>144304.88</v>
-      </c>
-      <c r="F29" t="n">
-        <v>3002.48</v>
-      </c>
-      <c r="G29" t="n">
-        <v>102.12</v>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>142102.40</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>138304.88</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>3797.52</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>97.33</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -1176,23 +1476,35 @@
           <t>30/08/2001</t>
         </is>
       </c>
-      <c r="B30" t="n">
-        <v>6000</v>
-      </c>
-      <c r="C30" t="n">
-        <v>147302.4</v>
-      </c>
-      <c r="D30" t="n">
-        <v>8000.8</v>
-      </c>
-      <c r="E30" t="n">
-        <v>152305.68</v>
-      </c>
-      <c r="F30" t="n">
-        <v>5003.28</v>
-      </c>
-      <c r="G30" t="n">
-        <v>103.4</v>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>6000.00</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>148102.40</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>8000.80</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>146305.68</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>1796.72</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>98.79</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -1201,23 +1513,35 @@
           <t>50/08/2000</t>
         </is>
       </c>
-      <c r="B31" t="n">
-        <v>3000.86</v>
-      </c>
-      <c r="C31" t="n">
-        <v>150303.26</v>
-      </c>
-      <c r="D31" t="n">
-        <v>6580.6</v>
-      </c>
-      <c r="E31" t="n">
-        <v>158886.28</v>
-      </c>
-      <c r="F31" t="n">
-        <v>8583.02</v>
-      </c>
-      <c r="G31" t="n">
-        <v>105.71</v>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>3000.86</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>151103.26</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>6580.60</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>152886.28</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>1783.02</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>101.18</t>
+        </is>
       </c>
     </row>
     <row r="32">
@@ -1233,7 +1557,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>185903.26</t>
+          <t>186703.26</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1243,17 +1567,17 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>223527.28</t>
+          <t>217527.28</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>37624.02</t>
+          <t>30824.02</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>120.24</t>
+          <t>116.51</t>
         </is>
       </c>
     </row>

</xml_diff>